<commit_message>
First pass at controller board layout
</commit_message>
<xml_diff>
--- a/excel/design_calculations.xlsx
+++ b/excel/design_calculations.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-checkouts\radar-speed-sign\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428E318F-7D18-4C0E-8ED7-9948FD9364ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2AC629-591D-4ADC-8F22-8CBA7AE0C1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39820" yWindow="1650" windowWidth="32090" windowHeight="15870" xr2:uid="{9B44D1DF-1120-4C84-A261-32B3BDD816A6}"/>
+    <workbookView xWindow="41900" yWindow="2580" windowWidth="32090" windowHeight="15870" activeTab="1" xr2:uid="{9B44D1DF-1120-4C84-A261-32B3BDD816A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bigass LED Calculations" sheetId="1" r:id="rId1"/>
+    <sheet name="Pico Board Calculations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Parameter</t>
   </si>
@@ -136,6 +137,30 @@
   </si>
   <si>
     <t>R_b</t>
+  </si>
+  <si>
+    <t>V_out</t>
+  </si>
+  <si>
+    <t>V_fb</t>
+  </si>
+  <si>
+    <t>R_bot</t>
+  </si>
+  <si>
+    <t>R_top</t>
+  </si>
+  <si>
+    <t>V_fb = V_out*(R_bot/(R_bot+R_top))</t>
+  </si>
+  <si>
+    <t>R_top = (V_out-V_fb)*R_bot/V_fb</t>
+  </si>
+  <si>
+    <t>V_fb*(R_bot+R_top) = V_out*R_bot</t>
+  </si>
+  <si>
+    <t>R_top = (V_out/V_fb-1)*R_bot</t>
   </si>
 </sst>
 </file>
@@ -143,7 +168,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -201,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -630,9 +655,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA6F0EE-19E6-4366-A6E8-3C79F2E40E87}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -869,4 +894,98 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE88844-D23D-4601-80EB-8BCD56A24E1B}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="16.83984375" customWidth="1"/>
+    <col min="2" max="2" width="9.15625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>1.23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="3">
+        <f>(B2/B3-1)*B4</f>
+        <v>30.650406504065046</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Make Rev C of segen seg, update README
</commit_message>
<xml_diff>
--- a/excel/design_calculations.xlsx
+++ b/excel/design_calculations.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-checkouts\radar-speed-sign\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2AC629-591D-4ADC-8F22-8CBA7AE0C1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5E5672-915B-4F5F-A5A0-EC56DB48BCB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41900" yWindow="2580" windowWidth="32090" windowHeight="15870" activeTab="1" xr2:uid="{9B44D1DF-1120-4C84-A261-32B3BDD816A6}"/>
+    <workbookView xWindow="2142" yWindow="192" windowWidth="20898" windowHeight="13488" activeTab="2" xr2:uid="{9B44D1DF-1120-4C84-A261-32B3BDD816A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bigass LED Calculations" sheetId="1" r:id="rId1"/>
     <sheet name="Pico Board Calculations" sheetId="2" r:id="rId2"/>
+    <sheet name="Horn Antenna" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
   <si>
     <t>Parameter</t>
   </si>
@@ -161,16 +162,92 @@
   </si>
   <si>
     <t>R_top = (V_out/V_fb-1)*R_bot</t>
+  </si>
+  <si>
+    <t>Near Field</t>
+  </si>
+  <si>
+    <t>c = f*lambda</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>GHz</t>
+  </si>
+  <si>
+    <t>d_k</t>
+  </si>
+  <si>
+    <t>Dielectric constant.</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>One wavelength. Everything closer than this is pretty much in the near field of the antenna and may affect its tuning.</t>
+  </si>
+  <si>
+    <t>Nickel Plating Cost Calculator</t>
+  </si>
+  <si>
+    <t>A_panel</t>
+  </si>
+  <si>
+    <t>Surface area of a single side panel.</t>
+  </si>
+  <si>
+    <t>mm^2</t>
+  </si>
+  <si>
+    <t>cm^2</t>
+  </si>
+  <si>
+    <t>Plating Thickness</t>
+  </si>
+  <si>
+    <t>Plating Time</t>
+  </si>
+  <si>
+    <t>um</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>Nickel Debits</t>
+  </si>
+  <si>
+    <t>A_total</t>
+  </si>
+  <si>
+    <t>mL</t>
+  </si>
+  <si>
+    <t>One-Plate Solution Volume</t>
+  </si>
+  <si>
+    <t>One-Plate Solution Cost/mL</t>
+  </si>
+  <si>
+    <t>Plating Solution Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,8 +271,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +289,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -218,11 +314,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -234,8 +331,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -900,7 +1001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE88844-D23D-4601-80EB-8BCD56A24E1B}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -988,4 +1089,190 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51592721-83AC-44D0-8642-1481CBCCA14B}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="25.41796875" customWidth="1"/>
+    <col min="2" max="2" width="9.15625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.41796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="7">
+        <f>300000000/(B5*1000000000)/B4*1000</f>
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9">
+        <v>3232.62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="7">
+        <f>B9/10/10</f>
+        <v>32.3262</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="7">
+        <f>8*B10</f>
+        <v>258.6096</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="9">
+        <f>B12/12.7*30</f>
+        <v>11.811023622047244</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="7">
+        <f>B11*0.155*B13</f>
+        <v>473.43883464566932</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="7">
+        <f>B14/6.08</f>
+        <v>77.868229382511402</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="7">
+        <f>44.99/946</f>
+        <v>4.755813953488372E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="8">
+        <f>B15*B16</f>
+        <v>3.7032681183078098</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update low pass filter and buffer code, README
* Low pass filter implemented on speed buffer.
* Speed buffer update interval added so that higher speeds (with more frequent rising edges) don't get knocked off the buffer too quickly.
* README updated with software update instructions.
</commit_message>
<xml_diff>
--- a/excel/design_calculations.xlsx
+++ b/excel/design_calculations.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git-checkouts\radar-speed-sign\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5E5672-915B-4F5F-A5A0-EC56DB48BCB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1CE1E0C-FAE5-4E03-8E55-5F823CC3CD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2142" yWindow="192" windowWidth="20898" windowHeight="13488" activeTab="2" xr2:uid="{9B44D1DF-1120-4C84-A261-32B3BDD816A6}"/>
+    <workbookView xWindow="-29590" yWindow="-3500" windowWidth="24620" windowHeight="9980" activeTab="3" xr2:uid="{9B44D1DF-1120-4C84-A261-32B3BDD816A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bigass LED Calculations" sheetId="1" r:id="rId1"/>
     <sheet name="Pico Board Calculations" sheetId="2" r:id="rId2"/>
     <sheet name="Horn Antenna" sheetId="3" r:id="rId3"/>
+    <sheet name="Radar Calibration" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
   <si>
     <t>Parameter</t>
   </si>
@@ -237,6 +239,27 @@
   </si>
   <si>
     <t>Plating Solution Cost</t>
+  </si>
+  <si>
+    <t>https://wx.erau.edu/faculty/mullerb/Wx365/Doppler_formulas/doppler_formulas.pdf</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>f_d</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>Doppler shift frequency.</t>
+  </si>
+  <si>
+    <t>Wavelength.</t>
+  </si>
+  <si>
+    <t>mph</t>
   </si>
 </sst>
 </file>
@@ -319,7 +342,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -334,6 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -446,6 +470,55 @@
         <a:xfrm>
           <a:off x="14084300" y="2946400"/>
           <a:ext cx="6142252" cy="4637172"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>248171</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>49829</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FC3432F-E1BC-79FB-D515-848510D0B04A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5414010" y="800100"/>
+          <a:ext cx="6008891" cy="3455969"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1095,7 +1168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51592721-83AC-44D0-8642-1481CBCCA14B}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1275,4 +1348,177 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083ABD29-2D30-44BD-9D98-642CCF09DBD8}">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="9.68359375" customWidth="1"/>
+    <col min="7" max="7" width="20.89453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
+        <v>10.525</v>
+      </c>
+      <c r="C2">
+        <v>10.525</v>
+      </c>
+      <c r="D2">
+        <v>10.525</v>
+      </c>
+      <c r="E2">
+        <v>10.525</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="10"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="7">
+        <f>300000000/(B2*1000000000)*1000</f>
+        <v>28.503562945368174</v>
+      </c>
+      <c r="C3" s="7">
+        <f>300000000/(C2*1000000000)*1000</f>
+        <v>28.503562945368174</v>
+      </c>
+      <c r="D3" s="7">
+        <f>300000000/(D2*1000000000)*1000</f>
+        <v>28.503562945368174</v>
+      </c>
+      <c r="E3" s="7">
+        <f>300000000/(E2*1000000000)*1000</f>
+        <v>28.503562945368174</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" s="10"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>35</v>
+      </c>
+      <c r="E4">
+        <v>95</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7">
+        <f>B4*0.44704</f>
+        <v>0.44703999999999999</v>
+      </c>
+      <c r="C5" s="7">
+        <f>C4*0.44704</f>
+        <v>2.2351999999999999</v>
+      </c>
+      <c r="D5" s="7">
+        <f>D4*0.44704</f>
+        <v>15.6464</v>
+      </c>
+      <c r="E5" s="7">
+        <f>E4*0.44704</f>
+        <v>42.468800000000002</v>
+      </c>
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="7">
+        <f>B5*2/(B3/1000)</f>
+        <v>31.367306666666664</v>
+      </c>
+      <c r="C6" s="7">
+        <f>C5*2/(C3/1000)</f>
+        <v>156.83653333333331</v>
+      </c>
+      <c r="D6" s="7">
+        <f>D5*2/(D3/1000)</f>
+        <v>1097.8557333333333</v>
+      </c>
+      <c r="E6" s="7">
+        <f>E5*2/(E3/1000)</f>
+        <v>2979.8941333333332</v>
+      </c>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{C6577223-FE23-4948-8672-5AB56A4918CC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>